<commit_message>
Adding translation to graphs in multiple languages based on Txt_translation_table.xlsx Correcting the Summary3_Filter with Extraction names
</commit_message>
<xml_diff>
--- a/Txt_translation_table.xlsx
+++ b/Txt_translation_table.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Documents\MINAGRIS_C\MINAGRIS_Microplastic_Soil_Assessmnent-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Documents\MINAGRIS_C\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8889B598-BD75-4170-952E-4918D516A5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8816FB60-429F-4721-B215-81CB4DA690E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7F2F662C-5BC8-4819-8CD3-426FFA89E794}"/>
+    <workbookView xWindow="10800" yWindow="-21600" windowWidth="29355" windowHeight="20985" xr2:uid="{7F2F662C-5BC8-4819-8CD3-426FFA89E794}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="73">
   <si>
     <t>All MINAGRIS, Micoplastic size distribution</t>
   </si>
@@ -105,13 +106,163 @@
   </si>
   <si>
     <t>Greec, CSS8</t>
+  </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Vsi MINAGRIS, velikosti mikroplastike (porazdelitev)</t>
+  </si>
+  <si>
+    <t>Vsi MINAGRIS, sestava polimerov mikroplastike</t>
+  </si>
+  <si>
+    <t>Vsi MINAGRIS, število delcev mikroplastike  na njivo</t>
+  </si>
+  <si>
+    <t>Povprečno število plastičnih delcev na kg tal</t>
+  </si>
+  <si>
+    <t>Velikostne kategorije [µm]</t>
+  </si>
+  <si>
+    <t>Druga plastika</t>
+  </si>
+  <si>
+    <t>Identificirani polimeri</t>
+  </si>
+  <si>
+    <t>All MINAGRIS, Microplastic particles per field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINAGRIS, Größenverteilung Mikroplastik </t>
+  </si>
+  <si>
+    <t>MINAGRIS, Mikroplastik Polymer-Zusammensetzung</t>
+  </si>
+  <si>
+    <t>MINAGRIS; Mikroplastik-Teilchen pro Feld</t>
+  </si>
+  <si>
+    <t>Durchschnittliche Anzahl von Mikroplastik-Teilchen pro kg Boden</t>
+  </si>
+  <si>
+    <t>Größenklassen [µm]</t>
+  </si>
+  <si>
+    <t>Anderes Plastik</t>
+  </si>
+  <si>
+    <t>identifizierte Polymere</t>
+  </si>
+  <si>
+    <t>Hist_Title_All</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pie_Title_All</t>
+  </si>
+  <si>
+    <t>Bar_Title_All</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hist_Title_CSS</t>
+  </si>
+  <si>
+    <t>Pie_Title_CSS</t>
+  </si>
+  <si>
+    <t>Bar_Title_CSS</t>
+  </si>
+  <si>
+    <t>y_nMiP_txt</t>
+  </si>
+  <si>
+    <t>Size_categories_txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Other_Plastic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Polymers_identified</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Slovenian</t>
+  </si>
+  <si>
+    <t>Dutch</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Estonian</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Austrian</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Italian</t>
+  </si>
+  <si>
+    <t>Greeck</t>
+  </si>
+  <si>
+    <t>Micoplastic size distribution</t>
+  </si>
+  <si>
+    <t>Microplastic polymer composition</t>
+  </si>
+  <si>
+    <t>Microplastic particles per field</t>
+  </si>
+  <si>
+    <t>Other Plastics</t>
+  </si>
+  <si>
+    <t>Mikroplasti osakest põllu kohta</t>
+  </si>
+  <si>
+    <t>Mikroplasti suuruse jaotus</t>
+  </si>
+  <si>
+    <t>Mikroplasti polümeeride koostis</t>
+  </si>
+  <si>
+    <t>število delcev mikroplastike  na njivo</t>
+  </si>
+  <si>
+    <t>sestava polimerov mikroplastike</t>
+  </si>
+  <si>
+    <t>velikosti mikroplastike (porazdelitev)</t>
+  </si>
+  <si>
+    <t>Mikroplastik Polymer-Zusammensetzung</t>
+  </si>
+  <si>
+    <t>Mikroplastik-Teilchen pro Feld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Größenverteilung Mikroplastik </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,13 +302,70 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="5">
@@ -224,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -240,6 +448,39 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,11 +794,495 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005D9A95-C845-4127-A670-194A5D90E2CE}">
+  <dimension ref="A1:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="28.44140625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="21.21875" style="15" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="15" customWidth="1"/>
+    <col min="9" max="9" width="31.77734375" style="15" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="8">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>5</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
+        <v>7</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
+        <v>8</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="13">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99D568ED-769B-47B3-8AF0-8994315F8782}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update the barplot from All minagris with  jitter and per CSS with black dot
</commit_message>
<xml_diff>
--- a/Txt_translation_table.xlsx
+++ b/Txt_translation_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Documents\MINAGRIS_C\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8816FB60-429F-4721-B215-81CB4DA690E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6168DDEE-D44B-4E50-ABAE-A8205241726E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10800" yWindow="-21600" windowWidth="29355" windowHeight="20985" xr2:uid="{7F2F662C-5BC8-4819-8CD3-426FFA89E794}"/>
+    <workbookView xWindow="-11670" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{7F2F662C-5BC8-4819-8CD3-426FFA89E794}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -153,9 +153,6 @@
     <t>Anderes Plastik</t>
   </si>
   <si>
-    <t>identifizierte Polymere</t>
-  </si>
-  <si>
     <t>Hist_Title_All</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t xml:space="preserve">Größenverteilung Mikroplastik </t>
+  </si>
+  <si>
+    <t>Identifizierte polymere</t>
   </si>
 </sst>
 </file>
@@ -798,7 +798,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,37 +821,37 @@
         <v>23</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -859,7 +859,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
@@ -871,13 +871,13 @@
         <v>31</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>6</v>
@@ -886,7 +886,7 @@
         <v>8</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>12</v>
@@ -897,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>24</v>
@@ -909,13 +909,13 @@
         <v>26</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I3" s="12" t="s">
         <v>27</v>
@@ -935,7 +935,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>0</v>
@@ -947,13 +947,13 @@
         <v>31</v>
       </c>
       <c r="F4" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>6</v>
@@ -962,7 +962,7 @@
         <v>8</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L4" s="14" t="s">
         <v>12</v>
@@ -973,7 +973,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>1</v>
@@ -985,13 +985,13 @@
         <v>5</v>
       </c>
       <c r="F5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>66</v>
-      </c>
       <c r="H5" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I5" s="16" t="s">
         <v>7</v>
@@ -1011,7 +1011,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>0</v>
@@ -1023,13 +1023,13 @@
         <v>31</v>
       </c>
       <c r="F6" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>6</v>
@@ -1038,7 +1038,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L6" s="14" t="s">
         <v>12</v>
@@ -1049,7 +1049,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>32</v>
@@ -1061,13 +1061,13 @@
         <v>34</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G7" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>70</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>71</v>
       </c>
       <c r="I7" s="17" t="s">
         <v>35</v>
@@ -1079,7 +1079,7 @@
         <v>37</v>
       </c>
       <c r="L7" s="17" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1087,7 +1087,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>0</v>
@@ -1099,13 +1099,13 @@
         <v>31</v>
       </c>
       <c r="F8" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>6</v>
@@ -1114,7 +1114,7 @@
         <v>8</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L8" s="14" t="s">
         <v>12</v>
@@ -1125,7 +1125,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>0</v>
@@ -1137,13 +1137,13 @@
         <v>31</v>
       </c>
       <c r="F9" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="H9" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>6</v>
@@ -1152,7 +1152,7 @@
         <v>8</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L9" s="14" t="s">
         <v>12</v>
@@ -1163,7 +1163,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>32</v>
@@ -1175,13 +1175,13 @@
         <v>34</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G10" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="15" t="s">
         <v>70</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>71</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>35</v>
@@ -1193,7 +1193,7 @@
         <v>37</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1201,7 +1201,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>0</v>
@@ -1213,13 +1213,13 @@
         <v>31</v>
       </c>
       <c r="F11" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="H11" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>6</v>
@@ -1228,7 +1228,7 @@
         <v>8</v>
       </c>
       <c r="K11" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L11" s="14" t="s">
         <v>12</v>
@@ -1239,7 +1239,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>0</v>
@@ -1251,13 +1251,13 @@
         <v>31</v>
       </c>
       <c r="F12" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="H12" s="14" t="s">
         <v>61</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>62</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>6</v>
@@ -1266,7 +1266,7 @@
         <v>8</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L12" s="14" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Update translation with /n when needed
</commit_message>
<xml_diff>
--- a/Txt_translation_table.xlsx
+++ b/Txt_translation_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Documents\MINAGRIS_C\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6168DDEE-D44B-4E50-ABAE-A8205241726E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE32B3A8-6C9C-4FC4-839A-FD99EC48FEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11670" yWindow="-21720" windowWidth="51840" windowHeight="21120" xr2:uid="{7F2F662C-5BC8-4819-8CD3-426FFA89E794}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7F2F662C-5BC8-4819-8CD3-426FFA89E794}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="74">
   <si>
     <t>All MINAGRIS, Micoplastic size distribution</t>
   </si>
@@ -144,9 +144,6 @@
     <t>MINAGRIS; Mikroplastik-Teilchen pro Feld</t>
   </si>
   <si>
-    <t>Durchschnittliche Anzahl von Mikroplastik-Teilchen pro kg Boden</t>
-  </si>
-  <si>
     <t>Größenklassen [µm]</t>
   </si>
   <si>
@@ -256,13 +253,38 @@
   </si>
   <si>
     <t>Identifizierte polymere</t>
+  </si>
+  <si>
+    <t>Nombre moyen de particules de plastic par kg de sol</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Durchschnittliche Anzahl von Mikroplastik-Teilchen </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>pro kg Boden</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,6 +360,12 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
@@ -448,17 +476,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -466,19 +485,28 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -798,477 +826,477 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="28.44140625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="21.21875" style="15" customWidth="1"/>
-    <col min="8" max="8" width="21.33203125" style="15" customWidth="1"/>
-    <col min="9" max="9" width="31.77734375" style="15" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="15"/>
+    <col min="1" max="1" width="4" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="28.44140625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" style="17" customWidth="1"/>
+    <col min="7" max="7" width="21.21875" style="17" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="17" customWidth="1"/>
+    <col min="9" max="9" width="31.77734375" style="17" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="17" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="14">
+        <v>3</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
+        <v>1</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="8">
+      <c r="C3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>2</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="17">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="E5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D6" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E6" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F6" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H6" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="L6" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="B7" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="L2" s="9" t="s">
+      <c r="K8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="10" t="s">
+    <row r="9" spans="1:12" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="17">
+        <v>9</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+      <c r="H10" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="14" t="s">
+      <c r="E11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E12" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H12" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="I12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="I4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="15">
-        <v>4</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
-        <v>5</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
-        <v>6</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
-        <v>7</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
-        <v>8</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="15">
-        <v>9</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" s="17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="13">
-        <v>10</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="13">
-        <v>11</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="L12" s="14" t="s">
+      <c r="L12" s="10" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New translations and saving graphs
</commit_message>
<xml_diff>
--- a/Txt_translation_table.xlsx
+++ b/Txt_translation_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Documents\MINAGRIS_C\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF065333-B254-4D06-818A-DF6A17C2C155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D999E26A-FAEB-45B5-8E21-E573438B3FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7F2F662C-5BC8-4819-8CD3-426FFA89E794}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="186">
   <si>
     <t>All MINAGRIS, Micoplastic size distribution</t>
   </si>
@@ -326,9 +326,6 @@
     <t>Nombre moyen de microplastiques par kg de sol</t>
   </si>
   <si>
-    <t>Durchschnittliche Anzahl von Mikroplastik \npro kg Boden</t>
-  </si>
-  <si>
     <t>Gemiddeld aantal microplastic per kg bodem</t>
   </si>
   <si>
@@ -464,9 +461,6 @@
     <t xml:space="preserve">MINAGRIS totaal, Samenstelling van microplastic polymeren </t>
   </si>
   <si>
-    <t xml:space="preserve">Totaal MINAGRIS, microplastic deeltjes </t>
-  </si>
-  <si>
     <t>Microplasticdeeltjes</t>
   </si>
   <si>
@@ -524,9 +518,6 @@
     <t>Λοιπά Πλαστικά</t>
   </si>
   <si>
-    <t>Πολυμερή που \nαναγνωρίστηκαν</t>
-  </si>
-  <si>
     <t>MINAGRIS, Distribution de la taille des microplastiques</t>
   </si>
   <si>
@@ -584,9 +575,6 @@
     <t>Número medio de partículas de plástico por kg de suelo</t>
   </si>
   <si>
-    <t>Categorías de tallas [µm]</t>
-  </si>
-  <si>
     <t>Catégories de taille [µm]</t>
   </si>
   <si>
@@ -605,14 +593,119 @@
     <t>In afwachting</t>
   </si>
   <si>
-    <t>Μέσος αριθμός μικροπλαστικών ανά \nχιλιόγραμμο εδάφους</t>
+    <r>
+      <t xml:space="preserve">Número medio de partículas de plástico </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>por kg de suelo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Μέσος αριθμός μικροπλαστικών ανά </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>χιλιόγραμμο εδάφους</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Durchschnittliche Anzahl von Mikroplastik </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>pro kg Boden</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Πολυμερή που </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>\n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>αναγνωρίστηκαν</t>
+    </r>
+  </si>
+  <si>
+    <t>Categorías de tamaño [µm]</t>
+  </si>
+  <si>
+    <t>Fortlaufende Analyse</t>
+  </si>
+  <si>
+    <t>Fehlende Bodenproben</t>
+  </si>
+  <si>
+    <t>Durschnittswert \naller Betriebe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MINAGRIS totaal , microplasticdeeltjes </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,8 +805,21 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,6 +859,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,7 +962,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -879,78 +991,86 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1269,30 +1389,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005D9A95-C845-4127-A670-194A5D90E2CE}">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4" style="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5546875" style="23" customWidth="1"/>
-    <col min="4" max="4" width="32.109375" style="23" customWidth="1"/>
-    <col min="5" max="5" width="28.44140625" style="23" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="23" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" style="23" customWidth="1"/>
-    <col min="9" max="9" width="18.88671875" style="23" customWidth="1"/>
-    <col min="10" max="11" width="20.6640625" style="23" customWidth="1"/>
-    <col min="12" max="12" width="28.109375" style="23" customWidth="1"/>
-    <col min="13" max="13" width="26.77734375" style="23" customWidth="1"/>
-    <col min="14" max="14" width="21.33203125" style="23" customWidth="1"/>
-    <col min="15" max="16" width="33.77734375" style="23" customWidth="1"/>
-    <col min="17" max="17" width="17.88671875" style="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" style="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="27.109375" style="23" customWidth="1"/>
-    <col min="20" max="16384" width="8.88671875" style="23"/>
+    <col min="1" max="1" width="4" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5546875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="28.44140625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" style="20" customWidth="1"/>
+    <col min="9" max="9" width="18.88671875" style="20" customWidth="1"/>
+    <col min="10" max="11" width="20.6640625" style="20" customWidth="1"/>
+    <col min="12" max="12" width="28.109375" style="20" customWidth="1"/>
+    <col min="13" max="13" width="26.77734375" style="20" customWidth="1"/>
+    <col min="14" max="14" width="21.33203125" style="20" customWidth="1"/>
+    <col min="15" max="15" width="39.88671875" style="20" customWidth="1"/>
+    <col min="16" max="16" width="33.77734375" style="20" customWidth="1"/>
+    <col min="17" max="17" width="23.5546875" style="20" customWidth="1"/>
+    <col min="18" max="18" width="13.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.5546875" style="20" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.88671875" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -1312,22 +1433,22 @@
         <v>36</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>37</v>
@@ -1354,7 +1475,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="13" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -1368,32 +1489,32 @@
         <v>25</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="G2" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>139</v>
-      </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="14" t="s">
+      <c r="H2" s="28" t="s">
+        <v>158</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="K2" s="28"/>
+      <c r="L2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="M2" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="N2" s="14" t="s">
-        <v>119</v>
+      <c r="N2" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="O2" s="11" t="s">
         <v>26</v>
@@ -1411,119 +1532,119 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="E3" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="K3" s="28"/>
+      <c r="L3" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>140</v>
-      </c>
-      <c r="J3" t="s">
-        <v>180</v>
-      </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="M3" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="N3" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="P3" s="18" t="s">
+      <c r="O3" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="P3" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="R3" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="S3" s="18" t="s">
+      <c r="S3" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="15">
+    <row r="4" spans="1:19" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="E4" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="G4" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="H4" s="20" t="s">
-        <v>125</v>
-      </c>
-      <c r="I4" s="20" t="s">
+      <c r="H4" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="J4" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="L4" s="21" t="s">
+      <c r="I4" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="N4" s="21" t="s">
-        <v>118</v>
-      </c>
-      <c r="O4" s="19" t="s">
+      <c r="N4" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="O4" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="21" t="s">
+      <c r="R4" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="S4" s="21" t="s">
+      <c r="S4" s="18" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1534,284 +1655,284 @@
       <c r="B5" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I5" s="13" t="s">
+      <c r="H5" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="J5" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="23" t="s">
+      <c r="I5" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="O5" s="22" t="s">
+      <c r="N5" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="O5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="P5" s="22" t="s">
+      <c r="P5" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="Q5" s="22" t="s">
+      <c r="Q5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="R5" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="22" t="s">
+      <c r="S5" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="E6" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G6" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="G6" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="K6" s="13"/>
-      <c r="L6" s="24" t="s">
+      <c r="H6" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="K6" s="28"/>
+      <c r="L6" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="25" t="s">
+      <c r="M6" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="N6" s="25" t="s">
-        <v>121</v>
-      </c>
-      <c r="O6" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="P6" s="26" t="s">
+      <c r="N6" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="O6" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="P6" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="Q6" s="27" t="s">
+      <c r="Q6" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="R6" s="27" t="s">
+      <c r="R6" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="S6" s="27" t="s">
-        <v>90</v>
+      <c r="S6" s="24" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+    <row r="7" spans="1:19" s="35" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="35">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="28" t="s">
+      <c r="D7" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="E7" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="J7" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="K7" s="13"/>
-      <c r="L7" s="23" t="s">
+      <c r="H7" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="I7" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="J7" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="K7" s="37"/>
+      <c r="L7" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="N7" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="O7" s="28" t="s">
+      <c r="N7" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="O7" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="P7" s="28" t="s">
+      <c r="P7" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="Q7" s="28" t="s">
+      <c r="Q7" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="R7" s="28" t="s">
+      <c r="R7" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="S7" s="28" t="s">
+      <c r="S7" s="36" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>7</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="E8" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="G8" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="H8" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="J8" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="K8" s="28"/>
+      <c r="L8" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="N8" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="O8" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="P8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q8" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="R8" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="S8" s="24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="15" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="F9" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="K8" s="13"/>
-      <c r="L8" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="M8" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="N8" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="O8" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="P8" s="27" t="s">
+      <c r="G9" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="H9" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="L9" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="N9" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="O9" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="P9" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="Q8" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="R8" s="27" t="s">
-        <v>83</v>
-      </c>
-      <c r="S8" s="27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="17">
-        <v>8</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="30" t="s">
-        <v>147</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="G9" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="H9" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>143</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="L9" s="30" t="s">
+      <c r="Q9" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="R9" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="M9" s="30" t="s">
-        <v>150</v>
-      </c>
-      <c r="N9" s="30" t="s">
-        <v>149</v>
-      </c>
-      <c r="O9" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="P9" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q9" s="26" t="s">
-        <v>152</v>
-      </c>
-      <c r="R9" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="S9" s="30" t="s">
-        <v>154</v>
+      <c r="S9" s="27" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
@@ -1821,182 +1942,182 @@
       <c r="B10" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="D10" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="28" t="s">
-        <v>112</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="E10" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="J10" s="36" t="s">
+      <c r="H10" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="I10" s="38" t="s">
+        <v>182</v>
+      </c>
+      <c r="J10" s="38" t="s">
+        <v>183</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="N10" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="O10" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="P10" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q10" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="M11" s="24" t="s">
+        <v>167</v>
+      </c>
+      <c r="N11" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="O11" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="P11" s="33" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="R11" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="S11" s="33" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="I12" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="J12" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="K12" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="L10" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="N10" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="O10" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="P10" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q10" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="R10" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="S10" s="28" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
-        <v>10</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="27" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>160</v>
-      </c>
-      <c r="F11" s="34" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="J11" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="K11" s="35" t="s">
+      <c r="L12" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="M12" s="24" t="s">
         <v>166</v>
       </c>
-      <c r="L11" s="27" t="s">
-        <v>167</v>
-      </c>
-      <c r="M11" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="N11" s="27" t="s">
+      <c r="N12" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="O12" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="P12" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q12" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="O11" t="s">
-        <v>173</v>
-      </c>
-      <c r="P11" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q11" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="R11" t="s">
-        <v>177</v>
-      </c>
-      <c r="S11" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" s="14" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
-        <v>11</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="27" t="s">
-        <v>155</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>158</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>159</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>108</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="J12" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="K12" s="35" t="s">
-        <v>165</v>
-      </c>
-      <c r="L12" s="27" t="s">
-        <v>168</v>
-      </c>
-      <c r="M12" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="N12" s="27" t="s">
+      <c r="R12" s="33" t="s">
         <v>172</v>
       </c>
-      <c r="O12" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="P12" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q12" s="27" t="s">
+      <c r="S12" s="33" t="s">
         <v>175</v>
-      </c>
-      <c r="R12" t="s">
-        <v>176</v>
-      </c>
-      <c r="S12" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="17" spans="8:11" x14ac:dyDescent="0.3">
-      <c r="H17" s="32"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="33"/>
+      <c r="H17" s="27"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
     </row>
     <row r="18" spans="8:11" x14ac:dyDescent="0.3">
-      <c r="H18" s="32"/>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33"/>
+      <c r="H18" s="27"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:S18" xr:uid="{005D9A95-C845-4127-A670-194A5D90E2CE}">
@@ -2134,7 +2255,7 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates Grpahs with Fileds instead of soil mean up to 4.1
</commit_message>
<xml_diff>
--- a/Txt_translation_table.xlsx
+++ b/Txt_translation_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berio001\Documents\MINAGRIS_C\MINAGRIS_Microplastic_Soil_Assessmnent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6F8BEB-D8C8-431A-B150-265C49DCE11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF16CFC-7455-418F-8AED-D89056AE8BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7F2F662C-5BC8-4819-8CD3-426FFA89E794}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="187">
   <si>
     <t>All MINAGRIS, Micoplastic size distribution</t>
   </si>
@@ -431,27 +431,9 @@
     <t>Field_sample</t>
   </si>
   <si>
-    <t>Average all farms</t>
-  </si>
-  <si>
-    <t>Individual \nfield sample</t>
-  </si>
-  <si>
     <t>Average_Farms</t>
   </si>
   <si>
-    <t>Moyenne des fermes</t>
-  </si>
-  <si>
-    <t>Echantillon unique</t>
-  </si>
-  <si>
-    <t>Monster</t>
-  </si>
-  <si>
-    <t>Muestra de campo</t>
-  </si>
-  <si>
     <t>Promedio todas fincas</t>
   </si>
   <si>
@@ -486,9 +468,6 @@
   </si>
   <si>
     <t>Δείγμα εδάφους που λείπει</t>
-  </si>
-  <si>
-    <t>Μεμονωμένο \nδείγμα αγρού</t>
   </si>
   <si>
     <t>Συνολικά MINAGRIS, Κατανομή μεγεθών μικροπλαστικών</t>
@@ -689,16 +668,40 @@
     <t>Fehlende Bodenproben</t>
   </si>
   <si>
-    <t>Durschnittswert \naller Betriebe</t>
-  </si>
-  <si>
     <t xml:space="preserve">MINAGRIS totaal , microplasticdeeltjes </t>
   </si>
   <si>
-    <t>Posamezni vzorec \njivo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gemiddelde van alle \nlandbouwbedrijven </t>
+  </si>
+  <si>
+    <t>Individual field</t>
+  </si>
+  <si>
+    <t>Veld</t>
+  </si>
+  <si>
+    <t>Njivo</t>
+  </si>
+  <si>
+    <t>Kohta</t>
+  </si>
+  <si>
+    <t>Feld</t>
+  </si>
+  <si>
+    <t>δείγμα</t>
+  </si>
+  <si>
+    <t>Cada Campo</t>
+  </si>
+  <si>
+    <t>Chaque champ</t>
+  </si>
+  <si>
+    <t>Average all fields</t>
+  </si>
+  <si>
+    <t>Moyenne des champs</t>
   </si>
 </sst>
 </file>
@@ -1389,8 +1392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{005D9A95-C845-4127-A670-194A5D90E2CE}">
   <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1442,13 +1445,13 @@
         <v>122</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>37</v>
@@ -1498,15 +1501,17 @@
         <v>96</v>
       </c>
       <c r="H2" s="28" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>137</v>
-      </c>
-      <c r="K2" s="28"/>
+        <v>131</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>132</v>
+      </c>
       <c r="L2" s="12" t="s">
         <v>60</v>
       </c>
@@ -1540,13 +1545,13 @@
         <v>45</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F3" s="30" t="s">
         <v>97</v>
@@ -1555,15 +1560,17 @@
         <v>98</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>128</v>
+        <v>178</v>
       </c>
       <c r="I3" s="28" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="J3" s="33" t="s">
-        <v>174</v>
-      </c>
-      <c r="K3" s="28"/>
+        <v>167</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>132</v>
+      </c>
       <c r="L3" s="16" t="s">
         <v>72</v>
       </c>
@@ -1571,7 +1578,7 @@
         <v>73</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="O3" s="14" t="s">
         <v>88</v>
@@ -1612,16 +1619,16 @@
         <v>94</v>
       </c>
       <c r="H4" s="31" t="s">
-        <v>124</v>
+        <v>177</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="K4" s="31" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="L4" s="18" t="s">
         <v>54</v>
@@ -1671,15 +1678,17 @@
         <v>100</v>
       </c>
       <c r="H5" s="28" t="s">
-        <v>124</v>
+        <v>180</v>
       </c>
       <c r="I5" s="28" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="K5" s="28"/>
+        <v>150</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>132</v>
+      </c>
       <c r="L5" s="20" t="s">
         <v>57</v>
       </c>
@@ -1728,15 +1737,17 @@
         <v>102</v>
       </c>
       <c r="H6" s="38" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I6" s="38" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J6" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="K6" s="28"/>
+        <v>174</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>132</v>
+      </c>
       <c r="L6" s="21" t="s">
         <v>62</v>
       </c>
@@ -1747,7 +1758,7 @@
         <v>120</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="P6" s="23" t="s">
         <v>67</v>
@@ -1785,15 +1796,17 @@
         <v>102</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I7" s="38" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J7" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="K7" s="37"/>
+        <v>174</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>132</v>
+      </c>
       <c r="L7" s="35" t="s">
         <v>62</v>
       </c>
@@ -1842,15 +1855,17 @@
         <v>104</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>124</v>
+        <v>177</v>
       </c>
       <c r="I8" s="28" t="s">
-        <v>123</v>
+        <v>185</v>
       </c>
       <c r="J8" s="29" t="s">
-        <v>157</v>
-      </c>
-      <c r="K8" s="28"/>
+        <v>150</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>132</v>
+      </c>
       <c r="L8" s="24" t="s">
         <v>80</v>
       </c>
@@ -1884,13 +1899,13 @@
         <v>53</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F9" s="32" t="s">
         <v>105</v>
@@ -1899,40 +1914,40 @@
         <v>105</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
       <c r="I9" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J9" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="L9" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="N9" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="J9" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="K9" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="L9" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="M9" s="27" t="s">
-        <v>147</v>
-      </c>
-      <c r="N9" s="27" t="s">
-        <v>146</v>
-      </c>
       <c r="O9" s="27" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="P9" s="23" t="s">
         <v>67</v>
       </c>
       <c r="Q9" s="23" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="R9" s="27" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="S9" s="27" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
@@ -1958,13 +1973,16 @@
         <v>102</v>
       </c>
       <c r="H10" s="38" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I10" s="38" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="J10" s="38" t="s">
-        <v>181</v>
+        <v>174</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>132</v>
       </c>
       <c r="L10" s="20" t="s">
         <v>62</v>
@@ -1999,13 +2017,13 @@
         <v>51</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="E11" s="24" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F11" s="28" t="s">
         <v>106</v>
@@ -2014,40 +2032,40 @@
         <v>109</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>129</v>
+        <v>183</v>
       </c>
       <c r="I11" s="28" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="J11" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="M11" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="N11" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="O11" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="P11" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="M11" s="24" t="s">
+      <c r="Q11" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="R11" s="33" t="s">
+        <v>164</v>
+      </c>
+      <c r="S11" s="33" t="s">
         <v>165</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="O11" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="P11" s="33" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q11" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="R11" s="33" t="s">
-        <v>171</v>
-      </c>
-      <c r="S11" s="33" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:19" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -2058,13 +2076,13 @@
         <v>50</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E12" s="24" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="F12" s="28" t="s">
         <v>107</v>
@@ -2073,25 +2091,25 @@
         <v>108</v>
       </c>
       <c r="H12" s="28" t="s">
-        <v>127</v>
+        <v>184</v>
       </c>
       <c r="I12" s="28" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="K12" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="M12" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="N12" s="24" t="s">
         <v>160</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="M12" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="N12" s="24" t="s">
-        <v>167</v>
       </c>
       <c r="O12" s="24" t="s">
         <v>87</v>
@@ -2100,13 +2118,13 @@
         <v>68</v>
       </c>
       <c r="Q12" s="24" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="R12" s="33" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="S12" s="33" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="8:11" x14ac:dyDescent="0.3">

</xml_diff>